<commit_message>
SCAN mode working, 32bit format unclear
</commit_message>
<xml_diff>
--- a/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
+++ b/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\STM32\cubeide\f373cc_psd_mirror_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687BA541-81BE-4691-816D-95A31C7EEC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B3DCD5-91BF-44C6-90E4-C241D47ED0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="4785" windowWidth="27660" windowHeight="15885" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
+    <workbookView xWindow="5670" yWindow="4680" windowWidth="37965" windowHeight="15885" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -813,7 +813,7 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="C7" s="7">
         <f>C6/C10</f>
-        <v>12.499491373697916</v>
+        <v>299.98779296875</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="F7" s="7">
         <f>1/C7</f>
-        <v>8.00032553407935E-2</v>
+        <v>3.3334689725330619E-3</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>7</v>
@@ -1103,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
@@ -1134,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="13">
-        <v>98304</v>
+        <v>4096</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="F10" s="12">
         <f>3*C11+(C12-1)*C11</f>
-        <v>99328</v>
+        <v>5120</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>5</v>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="F11" s="19">
         <f>F10*F6</f>
-        <v>8.0836622583926751E-2</v>
+        <v>4.166836215666327E-3</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>7</v>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="C12" s="15">
         <f>IF(C10&gt;512,C10/512,1)</f>
-        <v>192</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="3" t="s">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="F12" s="19">
         <f>1/F11</f>
-        <v>12.370630637886599</v>
+        <v>239.99023437500003</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>6</v>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C16" s="7">
         <f>F10*F6</f>
-        <v>8.0836622583926751E-2</v>
+        <v>4.166836215666327E-3</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="F16" s="17">
         <f>1/C16</f>
-        <v>12.370630637886599</v>
+        <v>239.99023437500003</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>6</v>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="C17" s="7">
         <f>(C16+F14)</f>
-        <v>8.0836622583926751E-2</v>
+        <v>4.166836215666327E-3</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>7</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C18" s="7">
         <f>C9*C17</f>
-        <v>8.0836622583926751E-2</v>
+        <v>1.6667344862665308E-2</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="C20" s="7">
         <f>C19-C18</f>
-        <v>0.91916337741607324</v>
+        <v>0.9833326551373347</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="C21" s="16">
         <f>C20/F6</f>
-        <v>1129422</v>
+        <v>1208270</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
SCAN mode working (polling IRQ pin)
</commit_message>
<xml_diff>
--- a/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
+++ b/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\STM32\cubeide\f373cc_psd_mirror_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B3DCD5-91BF-44C6-90E4-C241D47ED0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0C09D4-1B12-4C65-B3CD-DFE44F87C2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="4680" windowWidth="37965" windowHeight="15885" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
+    <workbookView xWindow="870" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1250,7 +1250,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="14">
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>5</v>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="F14" s="8">
         <f>C13*F6</f>
-        <v>0</v>
+        <v>4.1668362156663274E-4</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>7</v>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="C17" s="7">
         <f>(C16+F14)</f>
-        <v>4.166836215666327E-3</v>
+        <v>4.5835198372329595E-3</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>7</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C18" s="7">
         <f>C9*C17</f>
-        <v>1.6667344862665308E-2</v>
+        <v>1.8334079348931838E-2</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="C20" s="7">
         <f>C19-C18</f>
-        <v>0.9833326551373347</v>
+        <v>0.98166592065106817</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="C21" s="16">
         <f>C20/F6</f>
-        <v>1208270</v>
+        <v>1206222</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
SCAN mode via ISR working
</commit_message>
<xml_diff>
--- a/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
+++ b/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\STM32\cubeide\f373cc_psd_mirror_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0C09D4-1B12-4C65-B3CD-DFE44F87C2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6259C8D5-A538-4F74-B969-63B45C1DE725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
+    <workbookView xWindow="5385" yWindow="570" windowWidth="21600" windowHeight="10740" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -421,8 +421,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7086600" y="3028950"/>
-          <a:ext cx="6353175" cy="2076450"/>
+          <a:off x="7945531" y="3028950"/>
+          <a:ext cx="6308351" cy="1834403"/>
         </a:xfrm>
         <a:prstGeom prst="foldedCorner">
           <a:avLst/>
@@ -810,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75DC5B3-2DFD-4969-B8ED-6292D2990485}">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,6 +1589,156 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C14">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">

</xml_diff>

<commit_message>
first X/Y pattern readout from PSD working - no division by ambient light necessary??? - requires a lot of calibration - are voltage levels correct? - change gain resistors on PSD board?
</commit_message>
<xml_diff>
--- a/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
+++ b/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\STM32\cubeide\f373cc_psd_mirror_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6259C8D5-A538-4F74-B969-63B45C1DE725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2B4E7B-4281-499A-B43A-4555C348438E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="570" windowWidth="21600" windowHeight="10740" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -813,7 +813,7 @@
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z31" sqref="Z31"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="C7" s="7">
         <f>C6/C10</f>
-        <v>299.98779296875</v>
+        <v>599.9755859375</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="F7" s="7">
         <f>1/C7</f>
-        <v>3.3334689725330619E-3</v>
+        <v>1.666734486266531E-3</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>7</v>
@@ -1103,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
@@ -1134,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="13">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="F10" s="12">
         <f>3*C11+(C12-1)*C11</f>
-        <v>5120</v>
+        <v>3072</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>5</v>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="F11" s="19">
         <f>F10*F6</f>
-        <v>4.166836215666327E-3</v>
+        <v>2.5001017293997964E-3</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>7</v>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="C12" s="15">
         <f>IF(C10&gt;512,C10/512,1)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="3" t="s">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="F12" s="19">
         <f>1/F11</f>
-        <v>239.99023437500003</v>
+        <v>399.98372395833337</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>6</v>
@@ -1250,7 +1250,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="14">
-        <v>512</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>5</v>
@@ -1283,7 +1283,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="18">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="F14" s="8">
         <f>C13*F6</f>
-        <v>4.1668362156663274E-4</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>7</v>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C16" s="7">
         <f>F10*F6</f>
-        <v>4.166836215666327E-3</v>
+        <v>2.5001017293997964E-3</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="F16" s="17">
         <f>1/C16</f>
-        <v>239.99023437500003</v>
+        <v>399.98372395833337</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>6</v>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="C17" s="7">
         <f>(C16+F14)</f>
-        <v>4.5835198372329595E-3</v>
+        <v>2.5001017293997964E-3</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>7</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C18" s="7">
         <f>C9*C17</f>
-        <v>1.8334079348931838E-2</v>
+        <v>7.5003051881993889E-3</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="C19" s="7">
         <f>1/(C14)</f>
-        <v>1</v>
+        <v>7.6923076923076927E-3</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>7</v>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="C20" s="7">
         <f>C19-C18</f>
-        <v>0.98166592065106817</v>
+        <v>1.9200250410830386E-4</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="C21" s="16">
         <f>C20/F6</f>
-        <v>1206222</v>
+        <v>235.92307692307838</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>

</xml_diff>